<commit_message>
Added kAPI_RESULT_ENUM_CODE to APIs. Tried to fork matchUnits for grouping by unit, but gave up: should be a service for itself.
</commit_message>
<xml_diff>
--- a/Library/Templates/CWR_Inventory_Template.xlsx
+++ b/Library/Templates/CWR_Inventory_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="22300" windowHeight="16360" tabRatio="724"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="31760" windowHeight="21900" tabRatio="724"/>
   </bookViews>
   <sheets>
     <sheet name="IN_Identification" sheetId="10" r:id="rId1"/>
@@ -5922,8 +5922,8 @@
   <dimension ref="A1:BA8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="8" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7452,7 +7452,7 @@
   <dimension ref="A1:BR8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="8" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>